<commit_message>
- Add slider Menu
</commit_message>
<xml_diff>
--- a/Reports.xlsx
+++ b/Reports.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="20">
   <si>
     <t xml:space="preserve">Task</t>
   </si>
@@ -31,6 +31,12 @@
     <t xml:space="preserve">Status</t>
   </si>
   <si>
+    <t xml:space="preserve">Start Date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">End Date</t>
+  </si>
+  <si>
     <t xml:space="preserve">1. Dựng giao diện nib</t>
   </si>
   <si>
@@ -40,6 +46,9 @@
     <t xml:space="preserve">Done</t>
   </si>
   <si>
+    <t xml:space="preserve">21/12</t>
+  </si>
+  <si>
     <t xml:space="preserve">2. Thêm Debug Target</t>
   </si>
   <si>
@@ -50,6 +59,28 @@
   </si>
   <si>
     <t xml:space="preserve">4. Add CocoaPod</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5. Implement Alamofire</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.raywenderlich.com/147086/alamofire-tutorial-getting-started-2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">22/12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6. Implement Slider Menu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://cocoacasts.com/managing-view-controllers-with-container-view-controllers/
+https://www.raywenderlich.com/173544/ios-animation-tutorial-getting-started-3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25/12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">27/12</t>
   </si>
 </sst>
 </file>
@@ -131,13 +162,25 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -157,71 +200,138 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C5"/>
+  <dimension ref="B1:F7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
+      <selection pane="topLeft" activeCell="G10" activeCellId="0" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.04"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="68.37"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="68.37"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="5" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="B1" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="C1" s="0" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="D1" s="0" t="s">
         <v>2</v>
       </c>
+      <c r="E1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="0" t="s">
+      <c r="B2" s="0" t="s">
         <v>5</v>
       </c>
+      <c r="C2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>6</v>
-      </c>
       <c r="B3" s="0" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>5</v>
+        <v>10</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="0" t="s">
-        <v>5</v>
+      <c r="B4" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="0" t="s">
-        <v>5</v>
+      <c r="B5" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B6" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="49.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B7" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="https://www.weheartswift.com/remove-storyboard-from-project/"/>
+    <hyperlink ref="C2" r:id="rId1" display="https://www.weheartswift.com/remove-storyboard-from-project/"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>